<commit_message>
new bugfix for both ui and backend
</commit_message>
<xml_diff>
--- a/src/database/data/SummaryPayments.xlsx
+++ b/src/database/data/SummaryPayments.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D340BF-D7C2-43EC-BA61-E4E5206A91AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBBD971-4FD5-44F2-8B78-95BBB73DCB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRESCHOOL" sheetId="22" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="59">
   <si>
     <t>KINGSVILLE ADVANCED SCHOOLS SYSTEM</t>
   </si>
@@ -635,10 +635,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F1F01D-B476-4B73-B0ED-3675A6626318}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:BC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AI32" sqref="AI32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1194,17 +1197,7 @@
       </c>
     </row>
     <row r="31" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="32" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>25</v>
@@ -1223,6 +1216,7 @@
     <mergeCell ref="A4:AQ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>